<commit_message>
Changes in the AllSpace TestClass after integration
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/space_bulk_import.xlsx
+++ b/src/test/resources/testdata/space_bulk_import.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rehan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15135" windowHeight="2160"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -69,13 +65,13 @@
     <t>This is second bulk space</t>
   </si>
   <si>
-    <t>M-027</t>
-  </si>
-  <si>
-    <t>M-049</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>M-103</t>
+  </si>
+  <si>
+    <t>M-104</t>
   </si>
 </sst>
 </file>
@@ -208,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,7 +452,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +514,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -527,7 +523,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -553,13 +549,13 @@
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>